<commit_message>
Changes to board and code
</commit_message>
<xml_diff>
--- a/sputterizer.xlsx
+++ b/sputterizer.xlsx
@@ -181,7 +181,7 @@
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
@@ -190,7 +190,7 @@
     <col min="10" max="10" width="14" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
     <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="13" max="13" width="31" customWidth="1"/>
+    <col min="13" max="13" width="32" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
     <col min="15" max="15" width="16" customWidth="1"/>
     <col min="16" max="16" width="16" customWidth="1"/>
@@ -296,7 +296,7 @@
       </c>
       <c t="inlineStr" r="D2">
         <is>
-          <t/>
+          <t>Arduino_Nano_v3.x</t>
         </is>
       </c>
       <c t="inlineStr" r="E2">
@@ -326,7 +326,7 @@
         </is>
       </c>
       <c t="n" r="K2">
-        <v>1601</v>
+        <v>1451</v>
       </c>
       <c t="inlineStr" r="L2">
         <is>
@@ -372,7 +372,7 @@
       </c>
       <c t="inlineStr" r="D3">
         <is>
-          <t/>
+          <t>100nF</t>
         </is>
       </c>
       <c t="inlineStr" r="E3">
@@ -402,7 +402,7 @@
         </is>
       </c>
       <c t="n" r="K3">
-        <v>3069</v>
+        <v>2639</v>
       </c>
       <c t="inlineStr" r="L3">
         <is>
@@ -433,7 +433,7 @@
     <row r="4">
       <c t="inlineStr" r="A4">
         <is>
-          <t>25ML100MEFC8X7</t>
+          <t>35ML100MEFC8X7.5</t>
         </is>
       </c>
       <c t="inlineStr" r="B4">
@@ -443,12 +443,12 @@
       </c>
       <c t="inlineStr" r="C4">
         <is>
-          <t>1189-3982-ND</t>
+          <t>1189-4176-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D4">
         <is>
-          <t/>
+          <t>100uF</t>
         </is>
       </c>
       <c t="inlineStr" r="E4">
@@ -470,15 +470,15 @@
         <v>3</v>
       </c>
       <c t="n" r="I4">
-        <v>0.31000</v>
+        <v>0.42000</v>
       </c>
       <c t="inlineStr" r="J4">
         <is>
-          <t>$0.93</t>
+          <t>$1.26</t>
         </is>
       </c>
       <c t="n" r="K4">
-        <v>829</v>
+        <v>1772</v>
       </c>
       <c t="inlineStr" r="L4">
         <is>
@@ -487,7 +487,7 @@
       </c>
       <c t="inlineStr" r="M4">
         <is>
-          <t>CAP ALUM 100UF 20% 25V RADIAL</t>
+          <t>CAP ALUM 100UF 20% 35V RADIAL</t>
         </is>
       </c>
       <c t="inlineStr" r="N4">
@@ -524,7 +524,7 @@
       </c>
       <c t="inlineStr" r="D5">
         <is>
-          <t/>
+          <t>10nF</t>
         </is>
       </c>
       <c t="inlineStr" r="E5">
@@ -554,7 +554,7 @@
         </is>
       </c>
       <c t="n" r="K5">
-        <v>5950</v>
+        <v>5926</v>
       </c>
       <c t="inlineStr" r="L5">
         <is>
@@ -600,7 +600,7 @@
       </c>
       <c t="inlineStr" r="D6">
         <is>
-          <t/>
+          <t>100nF</t>
         </is>
       </c>
       <c t="inlineStr" r="E6">
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c t="n" r="K6">
-        <v>119308</v>
+        <v>115507</v>
       </c>
       <c t="inlineStr" r="L6">
         <is>
@@ -676,7 +676,7 @@
       </c>
       <c t="inlineStr" r="D7">
         <is>
-          <t/>
+          <t>1N4148</t>
         </is>
       </c>
       <c t="inlineStr" r="E7">
@@ -706,7 +706,7 @@
         </is>
       </c>
       <c t="n" r="K7">
-        <v>263154</v>
+        <v>245583</v>
       </c>
       <c t="inlineStr" r="L7">
         <is>
@@ -737,7 +737,7 @@
     <row r="8">
       <c t="inlineStr" r="A8">
         <is>
-          <t>151031SS04000</t>
+          <t>151031VS06000</t>
         </is>
       </c>
       <c t="inlineStr" r="B8">
@@ -747,12 +747,12 @@
       </c>
       <c t="inlineStr" r="C8">
         <is>
-          <t>732-5005-ND</t>
+          <t>732-5008-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D8">
         <is>
-          <t/>
+          <t>LED</t>
         </is>
       </c>
       <c t="inlineStr" r="E8">
@@ -774,15 +774,15 @@
         <v>1</v>
       </c>
       <c t="n" r="I8">
-        <v>0.17000</v>
+        <v>0.15000</v>
       </c>
       <c t="inlineStr" r="J8">
         <is>
-          <t>$0.17</t>
+          <t>$0.15</t>
         </is>
       </c>
       <c t="n" r="K8">
-        <v>5448</v>
+        <v>16916</v>
       </c>
       <c t="inlineStr" r="L8">
         <is>
@@ -791,7 +791,7 @@
       </c>
       <c t="inlineStr" r="M8">
         <is>
-          <t>LED RED DIFFUSED 3MM ROUND T/H</t>
+          <t>LED GREEN DIFFUSED 3MM ROUND T/H</t>
         </is>
       </c>
       <c t="inlineStr" r="N8">
@@ -828,7 +828,7 @@
       </c>
       <c t="inlineStr" r="D9">
         <is>
-          <t/>
+          <t>AudioJack2</t>
         </is>
       </c>
       <c t="inlineStr" r="E9">
@@ -858,7 +858,7 @@
         </is>
       </c>
       <c t="n" r="K9">
-        <v>115257</v>
+        <v>112149</v>
       </c>
       <c t="inlineStr" r="L9">
         <is>
@@ -904,7 +904,7 @@
       </c>
       <c t="inlineStr" r="D10">
         <is>
-          <t/>
+          <t>2X8 Header</t>
         </is>
       </c>
       <c t="inlineStr" r="E10">
@@ -934,7 +934,7 @@
         </is>
       </c>
       <c t="n" r="K10">
-        <v>3247</v>
+        <v>3214</v>
       </c>
       <c t="inlineStr" r="L10">
         <is>
@@ -980,7 +980,7 @@
       </c>
       <c t="inlineStr" r="D11">
         <is>
-          <t/>
+          <t>Conn_02x05_Odd_Even</t>
         </is>
       </c>
       <c t="inlineStr" r="E11">
@@ -1010,11 +1010,11 @@
         </is>
       </c>
       <c t="n" r="K11">
-        <v>26631</v>
+        <v>26153</v>
       </c>
       <c t="inlineStr" r="L11">
         <is>
-          <t>7 Weeks</t>
+          <t>9 Weeks</t>
         </is>
       </c>
       <c t="inlineStr" r="M11">
@@ -1056,7 +1056,7 @@
       </c>
       <c t="inlineStr" r="D12">
         <is>
-          <t/>
+          <t>Conn_01x02_Male</t>
         </is>
       </c>
       <c t="inlineStr" r="E12">
@@ -1086,7 +1086,7 @@
         </is>
       </c>
       <c t="n" r="K12">
-        <v>21670</v>
+        <v>20221</v>
       </c>
       <c t="inlineStr" r="L12">
         <is>
@@ -1132,7 +1132,7 @@
       </c>
       <c t="inlineStr" r="D13">
         <is>
-          <t/>
+          <t>LightPipe</t>
         </is>
       </c>
       <c t="inlineStr" r="E13">
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c t="n" r="K13">
-        <v>16015</v>
+        <v>15845</v>
       </c>
       <c t="inlineStr" r="L13">
         <is>
@@ -1193,32 +1193,32 @@
     <row r="14">
       <c t="inlineStr" r="A14">
         <is>
-          <t>CF14JT470R</t>
+          <t>BS170</t>
         </is>
       </c>
       <c t="inlineStr" r="B14">
         <is>
-          <t>Stackpole Electronics Inc</t>
+          <t>ON Semiconductor</t>
         </is>
       </c>
       <c t="inlineStr" r="C14">
         <is>
-          <t>CF14JT470RCT-ND</t>
+          <t>BS170-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D14">
         <is>
-          <t/>
+          <t>BS170</t>
         </is>
       </c>
       <c t="inlineStr" r="E14">
         <is>
-          <t>R1 R2 R3</t>
+          <t>Q1</t>
         </is>
       </c>
       <c t="inlineStr" r="F14">
         <is>
-          <t>Cut Tape (CT)</t>
+          <t>Bulk</t>
         </is>
       </c>
       <c t="inlineStr" r="G14">
@@ -1227,27 +1227,27 @@
         </is>
       </c>
       <c t="n" r="H14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c t="n" r="I14">
-        <v>0.10000</v>
+        <v>0.49000</v>
       </c>
       <c t="inlineStr" r="J14">
         <is>
-          <t>$0.30</t>
+          <t>$0.49</t>
         </is>
       </c>
       <c t="n" r="K14">
-        <v>228544</v>
+        <v>16133</v>
       </c>
       <c t="inlineStr" r="L14">
         <is>
-          <t>15 Weeks</t>
+          <t>6 Weeks</t>
         </is>
       </c>
       <c t="inlineStr" r="M14">
         <is>
-          <t>RES 470 OHM 1/4W 5% AXIAL</t>
+          <t>MOSFET N-CH 60V 500MA TO-92</t>
         </is>
       </c>
       <c t="inlineStr" r="N14">
@@ -1269,27 +1269,25 @@
     <row r="15">
       <c t="inlineStr" r="A15">
         <is>
-          <t>MRS25000C1002FCT00</t>
+          <t>CF14JT470R</t>
         </is>
       </c>
       <c t="inlineStr" r="B15">
         <is>
-          <t>Vishay BC Components</t>
+          <t>Stackpole Electronics Inc</t>
         </is>
       </c>
       <c t="inlineStr" r="C15">
         <is>
-          <t>BC3326CT-ND</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="D15">
-        <is>
-          <t/>
-        </is>
+          <t>CF14JT470RCT-ND</t>
+        </is>
+      </c>
+      <c t="n" r="D15">
+        <v>470</v>
       </c>
       <c t="inlineStr" r="E15">
         <is>
-          <t>R10 R9</t>
+          <t>R1 R2 R3</t>
         </is>
       </c>
       <c t="inlineStr" r="F15">
@@ -1303,27 +1301,27 @@
         </is>
       </c>
       <c t="n" r="H15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c t="n" r="I15">
-        <v>0.29000</v>
+        <v>0.10000</v>
       </c>
       <c t="inlineStr" r="J15">
         <is>
-          <t>$0.58</t>
+          <t>$0.30</t>
         </is>
       </c>
       <c t="n" r="K15">
-        <v>5551</v>
+        <v>344553</v>
       </c>
       <c t="inlineStr" r="L15">
         <is>
-          <t>16 Weeks</t>
+          <t>15 Weeks</t>
         </is>
       </c>
       <c t="inlineStr" r="M15">
         <is>
-          <t>RES 10K OHM 0.6W 1% AXIAL</t>
+          <t>RES 470 OHM 1/4W 5% AXIAL</t>
         </is>
       </c>
       <c t="inlineStr" r="N15">
@@ -1338,14 +1336,14 @@
       </c>
       <c t="inlineStr" r="P15">
         <is>
-          <t>Not Available</t>
+          <t>REACH Unaffected</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c t="inlineStr" r="A16">
         <is>
-          <t>MRS25000C1782FCT00</t>
+          <t>MRS25000C1002FCT00</t>
         </is>
       </c>
       <c t="inlineStr" r="B16">
@@ -1355,17 +1353,17 @@
       </c>
       <c t="inlineStr" r="C16">
         <is>
-          <t>BC4022CT-ND</t>
+          <t>BC3326CT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D16">
         <is>
-          <t/>
+          <t>10.0K</t>
         </is>
       </c>
       <c t="inlineStr" r="E16">
         <is>
-          <t>R4</t>
+          <t>R10 R9</t>
         </is>
       </c>
       <c t="inlineStr" r="F16">
@@ -1379,18 +1377,18 @@
         </is>
       </c>
       <c t="n" r="H16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c t="n" r="I16">
         <v>0.29000</v>
       </c>
       <c t="inlineStr" r="J16">
         <is>
-          <t>$0.29</t>
+          <t>$0.58</t>
         </is>
       </c>
       <c t="n" r="K16">
-        <v>14792</v>
+        <v>5562</v>
       </c>
       <c t="inlineStr" r="L16">
         <is>
@@ -1399,7 +1397,7 @@
       </c>
       <c t="inlineStr" r="M16">
         <is>
-          <t>RES 17.8K OHM 0.6W 1% AXIAL</t>
+          <t>RES 10K OHM 0.6W 1% AXIAL</t>
         </is>
       </c>
       <c t="inlineStr" r="N16">
@@ -1421,7 +1419,7 @@
     <row r="17">
       <c t="inlineStr" r="A17">
         <is>
-          <t>MRS25000C1403FCT00</t>
+          <t>MRS25000C1782FCT00</t>
         </is>
       </c>
       <c t="inlineStr" r="B17">
@@ -1431,17 +1429,17 @@
       </c>
       <c t="inlineStr" r="C17">
         <is>
-          <t>BC3995CT-ND</t>
+          <t>BC4022CT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D17">
         <is>
-          <t/>
+          <t>17.8K</t>
         </is>
       </c>
       <c t="inlineStr" r="E17">
         <is>
-          <t>R5</t>
+          <t>R4</t>
         </is>
       </c>
       <c t="inlineStr" r="F17">
@@ -1466,7 +1464,7 @@
         </is>
       </c>
       <c t="n" r="K17">
-        <v>4523</v>
+        <v>14789</v>
       </c>
       <c t="inlineStr" r="L17">
         <is>
@@ -1475,7 +1473,7 @@
       </c>
       <c t="inlineStr" r="M17">
         <is>
-          <t>RES 140K OHM 0.6W 1% AXIAL</t>
+          <t>RES 17.8K OHM 0.6W 1% AXIAL</t>
         </is>
       </c>
       <c t="inlineStr" r="N17">
@@ -1497,7 +1495,7 @@
     <row r="18">
       <c t="inlineStr" r="A18">
         <is>
-          <t>MRS25000C1582FCT00</t>
+          <t>MRS25000C1403FCT00</t>
         </is>
       </c>
       <c t="inlineStr" r="B18">
@@ -1507,17 +1505,17 @@
       </c>
       <c t="inlineStr" r="C18">
         <is>
-          <t>BC4574CT-ND</t>
+          <t>BC3995CT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D18">
         <is>
-          <t/>
+          <t>140K</t>
         </is>
       </c>
       <c t="inlineStr" r="E18">
         <is>
-          <t>R6</t>
+          <t>R5</t>
         </is>
       </c>
       <c t="inlineStr" r="F18">
@@ -1542,7 +1540,7 @@
         </is>
       </c>
       <c t="n" r="K18">
-        <v>3666</v>
+        <v>4520</v>
       </c>
       <c t="inlineStr" r="L18">
         <is>
@@ -1551,7 +1549,7 @@
       </c>
       <c t="inlineStr" r="M18">
         <is>
-          <t>RES 15.8K OHM 1% 0.6W AXIAL</t>
+          <t>RES 140K OHM 0.6W 1% AXIAL</t>
         </is>
       </c>
       <c t="inlineStr" r="N18">
@@ -1573,27 +1571,27 @@
     <row r="19">
       <c t="inlineStr" r="A19">
         <is>
-          <t>CF14JT1K00</t>
+          <t>MRS25000C1582FCT00</t>
         </is>
       </c>
       <c t="inlineStr" r="B19">
         <is>
-          <t>Stackpole Electronics Inc</t>
+          <t>Vishay BC Components</t>
         </is>
       </c>
       <c t="inlineStr" r="C19">
         <is>
-          <t>CF14JT1K00CT-ND</t>
+          <t>BC4574CT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D19">
         <is>
-          <t/>
+          <t>15.8K</t>
         </is>
       </c>
       <c t="inlineStr" r="E19">
         <is>
-          <t>R7</t>
+          <t>R6</t>
         </is>
       </c>
       <c t="inlineStr" r="F19">
@@ -1610,24 +1608,24 @@
         <v>1</v>
       </c>
       <c t="n" r="I19">
-        <v>0.10000</v>
+        <v>0.29000</v>
       </c>
       <c t="inlineStr" r="J19">
         <is>
-          <t>$0.10</t>
+          <t>$0.29</t>
         </is>
       </c>
       <c t="n" r="K19">
-        <v>899395</v>
+        <v>3663</v>
       </c>
       <c t="inlineStr" r="L19">
         <is>
-          <t>15 Weeks</t>
+          <t>16 Weeks</t>
         </is>
       </c>
       <c t="inlineStr" r="M19">
         <is>
-          <t>RES 1K OHM 1/4W 5% AXIAL</t>
+          <t>RES 15.8K OHM 1% 0.6W AXIAL</t>
         </is>
       </c>
       <c t="inlineStr" r="N19">
@@ -1642,14 +1640,14 @@
       </c>
       <c t="inlineStr" r="P19">
         <is>
-          <t>REACH Unaffected</t>
+          <t>Not Available</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c t="inlineStr" r="A20">
         <is>
-          <t>CF14JT10K0</t>
+          <t>CF14JT1K00</t>
         </is>
       </c>
       <c t="inlineStr" r="B20">
@@ -1659,17 +1657,17 @@
       </c>
       <c t="inlineStr" r="C20">
         <is>
-          <t>CF14JT10K0CT-ND</t>
+          <t>CF14JT1K00CT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D20">
         <is>
-          <t/>
+          <t>1K</t>
         </is>
       </c>
       <c t="inlineStr" r="E20">
         <is>
-          <t>R8</t>
+          <t>R7</t>
         </is>
       </c>
       <c t="inlineStr" r="F20">
@@ -1694,7 +1692,7 @@
         </is>
       </c>
       <c t="n" r="K20">
-        <v>1452231</v>
+        <v>806844</v>
       </c>
       <c t="inlineStr" r="L20">
         <is>
@@ -1703,7 +1701,7 @@
       </c>
       <c t="inlineStr" r="M20">
         <is>
-          <t>RES 10K OHM 1/4W 5% AXIAL</t>
+          <t>RES 1K OHM 1/4W 5% AXIAL</t>
         </is>
       </c>
       <c t="inlineStr" r="N20">
@@ -1725,226 +1723,378 @@
     <row r="21">
       <c t="inlineStr" r="A21">
         <is>
-          <t>PTV09A-2025F-B103</t>
+          <t>CF14JT10K0</t>
         </is>
       </c>
       <c t="inlineStr" r="B21">
         <is>
+          <t>Stackpole Electronics Inc</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C21">
+        <is>
+          <t>CF14JT10K0CT-ND</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="D21">
+        <is>
+          <t>10K</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="E21">
+        <is>
+          <t>R8</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F21">
+        <is>
+          <t>Cut Tape (CT)</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G21">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c t="n" r="H21">
+        <v>1</v>
+      </c>
+      <c t="n" r="I21">
+        <v>0.10000</v>
+      </c>
+      <c t="inlineStr" r="J21">
+        <is>
+          <t>$0.10</t>
+        </is>
+      </c>
+      <c t="n" r="K21">
+        <v>1273177</v>
+      </c>
+      <c t="inlineStr" r="L21">
+        <is>
+          <t>15 Weeks</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="M21">
+        <is>
+          <t>RES 10K OHM 1/4W 5% AXIAL</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="N21">
+        <is>
+          <t>RoHS Compliant</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="O21">
+        <is>
+          <t>Lead free</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="P21">
+        <is>
+          <t>REACH Unaffected</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c t="inlineStr" r="A22">
+        <is>
+          <t>PTD901-1015K-B103</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="B22">
+        <is>
           <t>Bourns Inc.</t>
         </is>
       </c>
-      <c t="inlineStr" r="C21">
-        <is>
-          <t>PTV09A-2025F-B103-ND</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="D21">
+      <c t="inlineStr" r="C22">
+        <is>
+          <t>PTD901-1015K-B103-ND</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="D22">
+        <is>
+          <t>10K</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="E22">
+        <is>
+          <t>RV1 RV2 RV3</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F22">
+        <is>
+          <t>Tray</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G22">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c t="n" r="H22">
+        <v>3</v>
+      </c>
+      <c t="n" r="I22">
+        <v>1.68000</v>
+      </c>
+      <c t="inlineStr" r="J22">
+        <is>
+          <t>$5.04</t>
+        </is>
+      </c>
+      <c t="n" r="K22">
+        <v>1139</v>
+      </c>
+      <c t="inlineStr" r="L22">
+        <is>
+          <t>16 Weeks</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="M22">
+        <is>
+          <t>POT 10K OHM 1/20W CARBON LINEAR</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="N22">
+        <is>
+          <t>RoHS Compliant</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="O22">
+        <is>
+          <t>Lead free</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="P22">
+        <is>
+          <t>REACH Unaffected</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c t="n" r="A23">
+        <v>5006</v>
+      </c>
+      <c t="inlineStr" r="B23">
+        <is>
+          <t>Keystone Electronics</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C23">
+        <is>
+          <t>36-5006-ND</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="D23">
+        <is>
+          <t>TestPoint</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="E23">
+        <is>
+          <t>TP1</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F23">
+        <is>
+          <t>Bulk</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G23">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c t="n" r="H23">
+        <v>1</v>
+      </c>
+      <c t="n" r="I23">
+        <v>0.35000</v>
+      </c>
+      <c t="inlineStr" r="J23">
+        <is>
+          <t>$0.35</t>
+        </is>
+      </c>
+      <c t="n" r="K23">
+        <v>209320</v>
+      </c>
+      <c t="inlineStr" r="L23">
+        <is>
+          <t>6 Weeks</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="M23">
+        <is>
+          <t>PC TEST POINT COMPACT BLACK</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="N23">
+        <is>
+          <t>RoHS Compliant</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="O23">
+        <is>
+          <t>Lead free</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="P23">
+        <is>
+          <t>REACH Unaffected</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c t="inlineStr" r="A24">
+        <is>
+          <t>SA5532AP</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="B24">
+        <is>
+          <t>Texas Instruments</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C24">
+        <is>
+          <t>296-16995-5-ND</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="D24">
+        <is>
+          <t>NE5532</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="E24">
+        <is>
+          <t>U1 U2</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F24">
+        <is>
+          <t>Tube</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G24">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c t="n" r="H24">
+        <v>2</v>
+      </c>
+      <c t="n" r="I24">
+        <v>0.94000</v>
+      </c>
+      <c t="inlineStr" r="J24">
+        <is>
+          <t>$1.88</t>
+        </is>
+      </c>
+      <c t="n" r="K24">
+        <v>3399</v>
+      </c>
+      <c t="inlineStr" r="L24">
+        <is>
+          <t>6 Weeks</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="M24">
+        <is>
+          <t>IC OPAMP GP 2 CIRCUIT 8DIP</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="N24">
+        <is>
+          <t>RoHS Compliant</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="O24">
+        <is>
+          <t>Lead free</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="P24">
+        <is>
+          <t>REACH Unaffected</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c t="inlineStr" r="A25">
+        <is>
+          <t>1221-L</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="B25">
+        <is>
+          <t>Davies Molding, LLC</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C25">
+        <is>
+          <t>1722-1314-ND</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="D25">
+        <is>
+          <t>Knob</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="E25">
         <is>
           <t/>
         </is>
       </c>
-      <c t="inlineStr" r="E21">
-        <is>
-          <t>RV1 RV2 RV3</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="F21">
-        <is>
-          <t>Tray</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="G21">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-      <c t="n" r="H21">
+      <c t="inlineStr" r="F25">
+        <is>
+          <t>Bulk</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G25">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c t="n" r="H25">
         <v>3</v>
       </c>
-      <c t="n" r="I21">
-        <v>0.83000</v>
-      </c>
-      <c t="inlineStr" r="J21">
-        <is>
-          <t>$2.49</t>
-        </is>
-      </c>
-      <c t="n" r="K21">
-        <v>25</v>
-      </c>
-      <c t="inlineStr" r="L21">
-        <is>
-          <t>18 Weeks</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="M21">
-        <is>
-          <t>POT 10K OHM 1/20W CARBON LINEAR</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="N21">
-        <is>
-          <t>RoHS Compliant</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="O21">
-        <is>
-          <t>Lead free</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="P21">
-        <is>
-          <t>REACH Unaffected</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c t="n" r="A22">
-        <v>5006</v>
-      </c>
-      <c t="inlineStr" r="B22">
-        <is>
-          <t>Keystone Electronics</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="C22">
-        <is>
-          <t>36-5006-ND</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="D22">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c t="inlineStr" r="E22">
-        <is>
-          <t>TP1</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="F22">
-        <is>
-          <t>Bulk</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="G22">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-      <c t="n" r="H22">
-        <v>1</v>
-      </c>
-      <c t="n" r="I22">
-        <v>0.35000</v>
-      </c>
-      <c t="inlineStr" r="J22">
-        <is>
-          <t>$0.35</t>
-        </is>
-      </c>
-      <c t="n" r="K22">
-        <v>219759</v>
-      </c>
-      <c t="inlineStr" r="L22">
+      <c t="n" r="I25">
+        <v>1.22000</v>
+      </c>
+      <c t="inlineStr" r="J25">
+        <is>
+          <t>$3.66</t>
+        </is>
+      </c>
+      <c t="n" r="K25">
+        <v>676</v>
+      </c>
+      <c t="inlineStr" r="L25">
         <is>
           <t>6 Weeks</t>
         </is>
       </c>
-      <c t="inlineStr" r="M22">
-        <is>
-          <t>PC TEST POINT COMPACT BLACK</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="N22">
-        <is>
-          <t>RoHS Compliant</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="O22">
-        <is>
-          <t>Lead free</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="P22">
-        <is>
-          <t>REACH Unaffected</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c t="inlineStr" r="A23">
-        <is>
-          <t>SA5532AP</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="B23">
-        <is>
-          <t>Texas Instruments</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="C23">
-        <is>
-          <t>296-16995-5-ND</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="D23">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c t="inlineStr" r="E23">
-        <is>
-          <t>U1 U2</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="F23">
-        <is>
-          <t>Tube</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="G23">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-      <c t="n" r="H23">
-        <v>2</v>
-      </c>
-      <c t="n" r="I23">
-        <v>0.94000</v>
-      </c>
-      <c t="inlineStr" r="J23">
-        <is>
-          <t>$1.88</t>
-        </is>
-      </c>
-      <c t="n" r="K23">
-        <v>3440</v>
-      </c>
-      <c t="inlineStr" r="L23">
-        <is>
-          <t>6 Weeks</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="M23">
-        <is>
-          <t>IC OPAMP GP 2 CIRCUIT 8DIP</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="N23">
-        <is>
-          <t>RoHS Compliant</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="O23">
-        <is>
-          <t>Lead free</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="P23">
-        <is>
-          <t>REACH Unaffected</t>
+      <c t="inlineStr" r="M25">
+        <is>
+          <t>KNOB SERRATED 0.236" PLASTIC</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="N25">
+        <is>
+          <t>RoHS Compliant</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="O25">
+        <is>
+          <t>Lead free</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="P25">
+        <is>
+          <t>Not Available</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
New design and code.
</commit_message>
<xml_diff>
--- a/sputterizer.xlsx
+++ b/sputterizer.xlsx
@@ -179,7 +179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="35" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
@@ -326,7 +326,7 @@
         </is>
       </c>
       <c t="n" r="K2">
-        <v>1451</v>
+        <v>1362</v>
       </c>
       <c t="inlineStr" r="L2">
         <is>
@@ -402,7 +402,7 @@
         </is>
       </c>
       <c t="n" r="K3">
-        <v>2639</v>
+        <v>1013</v>
       </c>
       <c t="inlineStr" r="L3">
         <is>
@@ -554,7 +554,7 @@
         </is>
       </c>
       <c t="n" r="K5">
-        <v>5926</v>
+        <v>5706</v>
       </c>
       <c t="inlineStr" r="L5">
         <is>
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c t="n" r="K6">
-        <v>115507</v>
+        <v>115422</v>
       </c>
       <c t="inlineStr" r="L6">
         <is>
@@ -706,7 +706,7 @@
         </is>
       </c>
       <c t="n" r="K7">
-        <v>245583</v>
+        <v>181978</v>
       </c>
       <c t="inlineStr" r="L7">
         <is>
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c t="n" r="K8">
-        <v>16916</v>
+        <v>16344</v>
       </c>
       <c t="inlineStr" r="L8">
         <is>
@@ -858,7 +858,7 @@
         </is>
       </c>
       <c t="n" r="K9">
-        <v>112149</v>
+        <v>106442</v>
       </c>
       <c t="inlineStr" r="L9">
         <is>
@@ -934,7 +934,7 @@
         </is>
       </c>
       <c t="n" r="K10">
-        <v>3214</v>
+        <v>3139</v>
       </c>
       <c t="inlineStr" r="L10">
         <is>
@@ -1010,7 +1010,7 @@
         </is>
       </c>
       <c t="n" r="K11">
-        <v>26153</v>
+        <v>25643</v>
       </c>
       <c t="inlineStr" r="L11">
         <is>
@@ -1086,7 +1086,7 @@
         </is>
       </c>
       <c t="n" r="K12">
-        <v>20221</v>
+        <v>17756</v>
       </c>
       <c t="inlineStr" r="L12">
         <is>
@@ -1117,32 +1117,32 @@
     <row r="13">
       <c t="inlineStr" r="A13">
         <is>
-          <t>7513D2-L</t>
+          <t>BS170</t>
         </is>
       </c>
       <c t="inlineStr" r="B13">
         <is>
-          <t>Visual Communications Company - VCC</t>
+          <t>ON Semiconductor</t>
         </is>
       </c>
       <c t="inlineStr" r="C13">
         <is>
-          <t>L71537-ND</t>
+          <t>BS170-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D13">
         <is>
-          <t>LightPipe</t>
+          <t>BS170</t>
         </is>
       </c>
       <c t="inlineStr" r="E13">
         <is>
-          <t>LP1</t>
+          <t>Q1</t>
         </is>
       </c>
       <c t="inlineStr" r="F13">
         <is>
-          <t>Bag</t>
+          <t>Bulk</t>
         </is>
       </c>
       <c t="inlineStr" r="G13">
@@ -1154,15 +1154,15 @@
         <v>1</v>
       </c>
       <c t="n" r="I13">
-        <v>0.63000</v>
+        <v>0.49000</v>
       </c>
       <c t="inlineStr" r="J13">
         <is>
-          <t>$0.63</t>
+          <t>$0.49</t>
         </is>
       </c>
       <c t="n" r="K13">
-        <v>15845</v>
+        <v>15875</v>
       </c>
       <c t="inlineStr" r="L13">
         <is>
@@ -1171,7 +1171,7 @@
       </c>
       <c t="inlineStr" r="M13">
         <is>
-          <t>LIGHT PIPE SGL RT ANGLE 3.6MM</t>
+          <t>MOSFET N-CH 60V 500MA TO-92</t>
         </is>
       </c>
       <c t="inlineStr" r="N13">
@@ -1193,32 +1193,30 @@
     <row r="14">
       <c t="inlineStr" r="A14">
         <is>
-          <t>BS170</t>
+          <t>CF14JT470R</t>
         </is>
       </c>
       <c t="inlineStr" r="B14">
         <is>
-          <t>ON Semiconductor</t>
+          <t>Stackpole Electronics Inc</t>
         </is>
       </c>
       <c t="inlineStr" r="C14">
         <is>
-          <t>BS170-ND</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="D14">
-        <is>
-          <t>BS170</t>
-        </is>
+          <t>CF14JT470RCT-ND</t>
+        </is>
+      </c>
+      <c t="n" r="D14">
+        <v>470</v>
       </c>
       <c t="inlineStr" r="E14">
         <is>
-          <t>Q1</t>
+          <t>R1 R2 R3</t>
         </is>
       </c>
       <c t="inlineStr" r="F14">
         <is>
-          <t>Bulk</t>
+          <t>Cut Tape (CT)</t>
         </is>
       </c>
       <c t="inlineStr" r="G14">
@@ -1227,27 +1225,27 @@
         </is>
       </c>
       <c t="n" r="H14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c t="n" r="I14">
-        <v>0.49000</v>
+        <v>0.10000</v>
       </c>
       <c t="inlineStr" r="J14">
         <is>
-          <t>$0.49</t>
+          <t>$0.30</t>
         </is>
       </c>
       <c t="n" r="K14">
-        <v>16133</v>
+        <v>337750</v>
       </c>
       <c t="inlineStr" r="L14">
         <is>
-          <t>6 Weeks</t>
+          <t>15 Weeks</t>
         </is>
       </c>
       <c t="inlineStr" r="M14">
         <is>
-          <t>MOSFET N-CH 60V 500MA TO-92</t>
+          <t>RES 470 OHM 1/4W 5% AXIAL</t>
         </is>
       </c>
       <c t="inlineStr" r="N14">
@@ -1269,25 +1267,27 @@
     <row r="15">
       <c t="inlineStr" r="A15">
         <is>
-          <t>CF14JT470R</t>
+          <t>MRS25000C1002FCT00</t>
         </is>
       </c>
       <c t="inlineStr" r="B15">
         <is>
-          <t>Stackpole Electronics Inc</t>
+          <t>Vishay BC Components</t>
         </is>
       </c>
       <c t="inlineStr" r="C15">
         <is>
-          <t>CF14JT470RCT-ND</t>
-        </is>
-      </c>
-      <c t="n" r="D15">
-        <v>470</v>
+          <t>BC3326CT-ND</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="D15">
+        <is>
+          <t>10.0K</t>
+        </is>
       </c>
       <c t="inlineStr" r="E15">
         <is>
-          <t>R1 R2 R3</t>
+          <t>R10 R9</t>
         </is>
       </c>
       <c t="inlineStr" r="F15">
@@ -1301,27 +1301,27 @@
         </is>
       </c>
       <c t="n" r="H15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c t="n" r="I15">
-        <v>0.10000</v>
+        <v>0.29000</v>
       </c>
       <c t="inlineStr" r="J15">
         <is>
-          <t>$0.30</t>
+          <t>$0.58</t>
         </is>
       </c>
       <c t="n" r="K15">
-        <v>344553</v>
+        <v>5562</v>
       </c>
       <c t="inlineStr" r="L15">
         <is>
-          <t>15 Weeks</t>
+          <t>16 Weeks</t>
         </is>
       </c>
       <c t="inlineStr" r="M15">
         <is>
-          <t>RES 470 OHM 1/4W 5% AXIAL</t>
+          <t>RES 10K OHM 0.6W 1% AXIAL</t>
         </is>
       </c>
       <c t="inlineStr" r="N15">
@@ -1336,14 +1336,14 @@
       </c>
       <c t="inlineStr" r="P15">
         <is>
-          <t>REACH Unaffected</t>
+          <t>Not Available</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c t="inlineStr" r="A16">
         <is>
-          <t>MRS25000C1002FCT00</t>
+          <t>MRS25000C1782FCT00</t>
         </is>
       </c>
       <c t="inlineStr" r="B16">
@@ -1353,17 +1353,17 @@
       </c>
       <c t="inlineStr" r="C16">
         <is>
-          <t>BC3326CT-ND</t>
+          <t>BC4022CT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D16">
         <is>
-          <t>10.0K</t>
+          <t>17.8K</t>
         </is>
       </c>
       <c t="inlineStr" r="E16">
         <is>
-          <t>R10 R9</t>
+          <t>R4</t>
         </is>
       </c>
       <c t="inlineStr" r="F16">
@@ -1377,18 +1377,18 @@
         </is>
       </c>
       <c t="n" r="H16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c t="n" r="I16">
         <v>0.29000</v>
       </c>
       <c t="inlineStr" r="J16">
         <is>
-          <t>$0.58</t>
+          <t>$0.29</t>
         </is>
       </c>
       <c t="n" r="K16">
-        <v>5562</v>
+        <v>14785</v>
       </c>
       <c t="inlineStr" r="L16">
         <is>
@@ -1397,7 +1397,7 @@
       </c>
       <c t="inlineStr" r="M16">
         <is>
-          <t>RES 10K OHM 0.6W 1% AXIAL</t>
+          <t>RES 17.8K OHM 0.6W 1% AXIAL</t>
         </is>
       </c>
       <c t="inlineStr" r="N16">
@@ -1419,7 +1419,7 @@
     <row r="17">
       <c t="inlineStr" r="A17">
         <is>
-          <t>MRS25000C1782FCT00</t>
+          <t>MRS25000C1403FCT00</t>
         </is>
       </c>
       <c t="inlineStr" r="B17">
@@ -1429,17 +1429,17 @@
       </c>
       <c t="inlineStr" r="C17">
         <is>
-          <t>BC4022CT-ND</t>
+          <t>BC3995CT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D17">
         <is>
-          <t>17.8K</t>
+          <t>140K</t>
         </is>
       </c>
       <c t="inlineStr" r="E17">
         <is>
-          <t>R4</t>
+          <t>R5</t>
         </is>
       </c>
       <c t="inlineStr" r="F17">
@@ -1464,7 +1464,7 @@
         </is>
       </c>
       <c t="n" r="K17">
-        <v>14789</v>
+        <v>4495</v>
       </c>
       <c t="inlineStr" r="L17">
         <is>
@@ -1473,7 +1473,7 @@
       </c>
       <c t="inlineStr" r="M17">
         <is>
-          <t>RES 17.8K OHM 0.6W 1% AXIAL</t>
+          <t>RES 140K OHM 0.6W 1% AXIAL</t>
         </is>
       </c>
       <c t="inlineStr" r="N17">
@@ -1495,7 +1495,7 @@
     <row r="18">
       <c t="inlineStr" r="A18">
         <is>
-          <t>MRS25000C1403FCT00</t>
+          <t>MRS25000C1582FCT00</t>
         </is>
       </c>
       <c t="inlineStr" r="B18">
@@ -1505,17 +1505,17 @@
       </c>
       <c t="inlineStr" r="C18">
         <is>
-          <t>BC3995CT-ND</t>
+          <t>BC4574CT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D18">
         <is>
-          <t>140K</t>
+          <t>15.8K</t>
         </is>
       </c>
       <c t="inlineStr" r="E18">
         <is>
-          <t>R5</t>
+          <t>R6</t>
         </is>
       </c>
       <c t="inlineStr" r="F18">
@@ -1540,7 +1540,7 @@
         </is>
       </c>
       <c t="n" r="K18">
-        <v>4520</v>
+        <v>3663</v>
       </c>
       <c t="inlineStr" r="L18">
         <is>
@@ -1549,7 +1549,7 @@
       </c>
       <c t="inlineStr" r="M18">
         <is>
-          <t>RES 140K OHM 0.6W 1% AXIAL</t>
+          <t>RES 15.8K OHM 1% 0.6W AXIAL</t>
         </is>
       </c>
       <c t="inlineStr" r="N18">
@@ -1571,27 +1571,27 @@
     <row r="19">
       <c t="inlineStr" r="A19">
         <is>
-          <t>MRS25000C1582FCT00</t>
+          <t>CF14JT1K00</t>
         </is>
       </c>
       <c t="inlineStr" r="B19">
         <is>
-          <t>Vishay BC Components</t>
+          <t>Stackpole Electronics Inc</t>
         </is>
       </c>
       <c t="inlineStr" r="C19">
         <is>
-          <t>BC4574CT-ND</t>
+          <t>CF14JT1K00CT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D19">
         <is>
-          <t>15.8K</t>
+          <t>1K</t>
         </is>
       </c>
       <c t="inlineStr" r="E19">
         <is>
-          <t>R6</t>
+          <t>R7</t>
         </is>
       </c>
       <c t="inlineStr" r="F19">
@@ -1608,24 +1608,24 @@
         <v>1</v>
       </c>
       <c t="n" r="I19">
-        <v>0.29000</v>
+        <v>0.10000</v>
       </c>
       <c t="inlineStr" r="J19">
         <is>
-          <t>$0.29</t>
+          <t>$0.10</t>
         </is>
       </c>
       <c t="n" r="K19">
-        <v>3663</v>
+        <v>791941</v>
       </c>
       <c t="inlineStr" r="L19">
         <is>
-          <t>16 Weeks</t>
+          <t>15 Weeks</t>
         </is>
       </c>
       <c t="inlineStr" r="M19">
         <is>
-          <t>RES 15.8K OHM 1% 0.6W AXIAL</t>
+          <t>RES 1K OHM 1/4W 5% AXIAL</t>
         </is>
       </c>
       <c t="inlineStr" r="N19">
@@ -1640,14 +1640,14 @@
       </c>
       <c t="inlineStr" r="P19">
         <is>
-          <t>Not Available</t>
+          <t>REACH Unaffected</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c t="inlineStr" r="A20">
         <is>
-          <t>CF14JT1K00</t>
+          <t>CF14JT10K0</t>
         </is>
       </c>
       <c t="inlineStr" r="B20">
@@ -1657,17 +1657,17 @@
       </c>
       <c t="inlineStr" r="C20">
         <is>
-          <t>CF14JT1K00CT-ND</t>
+          <t>CF14JT10K0CT-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D20">
         <is>
-          <t>1K</t>
+          <t>10K</t>
         </is>
       </c>
       <c t="inlineStr" r="E20">
         <is>
-          <t>R7</t>
+          <t>R8</t>
         </is>
       </c>
       <c t="inlineStr" r="F20">
@@ -1692,7 +1692,7 @@
         </is>
       </c>
       <c t="n" r="K20">
-        <v>806844</v>
+        <v>1333942</v>
       </c>
       <c t="inlineStr" r="L20">
         <is>
@@ -1701,7 +1701,7 @@
       </c>
       <c t="inlineStr" r="M20">
         <is>
-          <t>RES 1K OHM 1/4W 5% AXIAL</t>
+          <t>RES 10K OHM 1/4W 5% AXIAL</t>
         </is>
       </c>
       <c t="inlineStr" r="N20">
@@ -1723,17 +1723,17 @@
     <row r="21">
       <c t="inlineStr" r="A21">
         <is>
-          <t>CF14JT10K0</t>
+          <t>PTD901-1015K-B103</t>
         </is>
       </c>
       <c t="inlineStr" r="B21">
         <is>
-          <t>Stackpole Electronics Inc</t>
+          <t>Bourns Inc.</t>
         </is>
       </c>
       <c t="inlineStr" r="C21">
         <is>
-          <t>CF14JT10K0CT-ND</t>
+          <t>PTD901-1015K-B103-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D21">
@@ -1743,12 +1743,12 @@
       </c>
       <c t="inlineStr" r="E21">
         <is>
-          <t>R8</t>
+          <t>RV1 RV2 RV3</t>
         </is>
       </c>
       <c t="inlineStr" r="F21">
         <is>
-          <t>Cut Tape (CT)</t>
+          <t>Tray</t>
         </is>
       </c>
       <c t="inlineStr" r="G21">
@@ -1757,148 +1757,148 @@
         </is>
       </c>
       <c t="n" r="H21">
+        <v>3</v>
+      </c>
+      <c t="n" r="I21">
+        <v>1.68000</v>
+      </c>
+      <c t="inlineStr" r="J21">
+        <is>
+          <t>$5.04</t>
+        </is>
+      </c>
+      <c t="n" r="K21">
+        <v>1139</v>
+      </c>
+      <c t="inlineStr" r="L21">
+        <is>
+          <t>16 Weeks</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="M21">
+        <is>
+          <t>POT 10K OHM 1/20W CARBON LINEAR</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="N21">
+        <is>
+          <t>RoHS Compliant</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="O21">
+        <is>
+          <t>Lead free</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="P21">
+        <is>
+          <t>REACH Unaffected</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c t="n" r="A22">
+        <v>5006</v>
+      </c>
+      <c t="inlineStr" r="B22">
+        <is>
+          <t>Keystone Electronics</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C22">
+        <is>
+          <t>36-5006-ND</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="D22">
+        <is>
+          <t>TestPoint</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="E22">
+        <is>
+          <t>TP1</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F22">
+        <is>
+          <t>Bulk</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G22">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c t="n" r="H22">
         <v>1</v>
       </c>
-      <c t="n" r="I21">
-        <v>0.10000</v>
-      </c>
-      <c t="inlineStr" r="J21">
-        <is>
-          <t>$0.10</t>
-        </is>
-      </c>
-      <c t="n" r="K21">
-        <v>1273177</v>
-      </c>
-      <c t="inlineStr" r="L21">
-        <is>
-          <t>15 Weeks</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="M21">
-        <is>
-          <t>RES 10K OHM 1/4W 5% AXIAL</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="N21">
-        <is>
-          <t>RoHS Compliant</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="O21">
-        <is>
-          <t>Lead free</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="P21">
+      <c t="n" r="I22">
+        <v>0.35000</v>
+      </c>
+      <c t="inlineStr" r="J22">
+        <is>
+          <t>$0.35</t>
+        </is>
+      </c>
+      <c t="n" r="K22">
+        <v>199128</v>
+      </c>
+      <c t="inlineStr" r="L22">
+        <is>
+          <t>6 Weeks</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="M22">
+        <is>
+          <t>PC TEST POINT COMPACT BLACK</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="N22">
+        <is>
+          <t>RoHS Compliant</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="O22">
+        <is>
+          <t>Lead free</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="P22">
         <is>
           <t>REACH Unaffected</t>
         </is>
       </c>
     </row>
-    <row r="22">
-      <c t="inlineStr" r="A22">
-        <is>
-          <t>PTD901-1015K-B103</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="B22">
-        <is>
-          <t>Bourns Inc.</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="C22">
-        <is>
-          <t>PTD901-1015K-B103-ND</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="D22">
-        <is>
-          <t>10K</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="E22">
-        <is>
-          <t>RV1 RV2 RV3</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="F22">
-        <is>
-          <t>Tray</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="G22">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-      <c t="n" r="H22">
-        <v>3</v>
-      </c>
-      <c t="n" r="I22">
-        <v>1.68000</v>
-      </c>
-      <c t="inlineStr" r="J22">
-        <is>
-          <t>$5.04</t>
-        </is>
-      </c>
-      <c t="n" r="K22">
-        <v>1139</v>
-      </c>
-      <c t="inlineStr" r="L22">
-        <is>
-          <t>16 Weeks</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="M22">
-        <is>
-          <t>POT 10K OHM 1/20W CARBON LINEAR</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="N22">
-        <is>
-          <t>RoHS Compliant</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="O22">
-        <is>
-          <t>Lead free</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="P22">
-        <is>
-          <t>REACH Unaffected</t>
-        </is>
-      </c>
-    </row>
     <row r="23">
-      <c t="n" r="A23">
-        <v>5006</v>
+      <c t="inlineStr" r="A23">
+        <is>
+          <t>SA5532AP</t>
+        </is>
       </c>
       <c t="inlineStr" r="B23">
         <is>
-          <t>Keystone Electronics</t>
+          <t>Texas Instruments</t>
         </is>
       </c>
       <c t="inlineStr" r="C23">
         <is>
-          <t>36-5006-ND</t>
+          <t>296-16995-5-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D23">
         <is>
-          <t>TestPoint</t>
+          <t>NE5532</t>
         </is>
       </c>
       <c t="inlineStr" r="E23">
         <is>
-          <t>TP1</t>
+          <t>U1 U2</t>
         </is>
       </c>
       <c t="inlineStr" r="F23">
         <is>
-          <t>Bulk</t>
+          <t>Tube</t>
         </is>
       </c>
       <c t="inlineStr" r="G23">
@@ -1907,18 +1907,18 @@
         </is>
       </c>
       <c t="n" r="H23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c t="n" r="I23">
-        <v>0.35000</v>
+        <v>0.94000</v>
       </c>
       <c t="inlineStr" r="J23">
         <is>
-          <t>$0.35</t>
+          <t>$1.88</t>
         </is>
       </c>
       <c t="n" r="K23">
-        <v>209320</v>
+        <v>3384</v>
       </c>
       <c t="inlineStr" r="L23">
         <is>
@@ -1927,7 +1927,7 @@
       </c>
       <c t="inlineStr" r="M23">
         <is>
-          <t>PC TEST POINT COMPACT BLACK</t>
+          <t>IC OPAMP GP 2 CIRCUIT 8DIP</t>
         </is>
       </c>
       <c t="inlineStr" r="N23">
@@ -1949,32 +1949,32 @@
     <row r="24">
       <c t="inlineStr" r="A24">
         <is>
-          <t>SA5532AP</t>
+          <t>1221-L</t>
         </is>
       </c>
       <c t="inlineStr" r="B24">
         <is>
-          <t>Texas Instruments</t>
+          <t>Davies Molding, LLC</t>
         </is>
       </c>
       <c t="inlineStr" r="C24">
         <is>
-          <t>296-16995-5-ND</t>
+          <t>1722-1314-ND</t>
         </is>
       </c>
       <c t="inlineStr" r="D24">
         <is>
-          <t>NE5532</t>
+          <t>Knob</t>
         </is>
       </c>
       <c t="inlineStr" r="E24">
         <is>
-          <t>U1 U2</t>
+          <t/>
         </is>
       </c>
       <c t="inlineStr" r="F24">
         <is>
-          <t>Tube</t>
+          <t>Bulk</t>
         </is>
       </c>
       <c t="inlineStr" r="G24">
@@ -1983,18 +1983,18 @@
         </is>
       </c>
       <c t="n" r="H24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c t="n" r="I24">
-        <v>0.94000</v>
+        <v>1.22000</v>
       </c>
       <c t="inlineStr" r="J24">
         <is>
-          <t>$1.88</t>
+          <t>$3.66</t>
         </is>
       </c>
       <c t="n" r="K24">
-        <v>3399</v>
+        <v>676</v>
       </c>
       <c t="inlineStr" r="L24">
         <is>
@@ -2003,7 +2003,7 @@
       </c>
       <c t="inlineStr" r="M24">
         <is>
-          <t>IC OPAMP GP 2 CIRCUIT 8DIP</t>
+          <t>KNOB SERRATED 0.236" PLASTIC</t>
         </is>
       </c>
       <c t="inlineStr" r="N24">
@@ -2017,82 +2017,6 @@
         </is>
       </c>
       <c t="inlineStr" r="P24">
-        <is>
-          <t>REACH Unaffected</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c t="inlineStr" r="A25">
-        <is>
-          <t>1221-L</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="B25">
-        <is>
-          <t>Davies Molding, LLC</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="C25">
-        <is>
-          <t>1722-1314-ND</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="D25">
-        <is>
-          <t>Knob</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="E25">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c t="inlineStr" r="F25">
-        <is>
-          <t>Bulk</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="G25">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-      <c t="n" r="H25">
-        <v>3</v>
-      </c>
-      <c t="n" r="I25">
-        <v>1.22000</v>
-      </c>
-      <c t="inlineStr" r="J25">
-        <is>
-          <t>$3.66</t>
-        </is>
-      </c>
-      <c t="n" r="K25">
-        <v>676</v>
-      </c>
-      <c t="inlineStr" r="L25">
-        <is>
-          <t>6 Weeks</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="M25">
-        <is>
-          <t>KNOB SERRATED 0.236" PLASTIC</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="N25">
-        <is>
-          <t>RoHS Compliant</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="O25">
-        <is>
-          <t>Lead free</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="P25">
         <is>
           <t>Not Available</t>
         </is>

</xml_diff>

<commit_message>
New code and BOM
</commit_message>
<xml_diff>
--- a/sputterizer.xlsx
+++ b/sputterizer.xlsx
@@ -326,7 +326,7 @@
         </is>
       </c>
       <c t="n" r="K2">
-        <v>1362</v>
+        <v>1217</v>
       </c>
       <c t="inlineStr" r="L2">
         <is>
@@ -402,7 +402,7 @@
         </is>
       </c>
       <c t="n" r="K3">
-        <v>1013</v>
+        <v>0</v>
       </c>
       <c t="inlineStr" r="L3">
         <is>
@@ -478,11 +478,11 @@
         </is>
       </c>
       <c t="n" r="K4">
-        <v>1772</v>
+        <v>1753</v>
       </c>
       <c t="inlineStr" r="L4">
         <is>
-          <t>17 Weeks</t>
+          <t>16 Weeks</t>
         </is>
       </c>
       <c t="inlineStr" r="M4">
@@ -554,7 +554,7 @@
         </is>
       </c>
       <c t="n" r="K5">
-        <v>5706</v>
+        <v>3703</v>
       </c>
       <c t="inlineStr" r="L5">
         <is>
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c t="n" r="K6">
-        <v>115422</v>
+        <v>115394</v>
       </c>
       <c t="inlineStr" r="L6">
         <is>
@@ -706,7 +706,7 @@
         </is>
       </c>
       <c t="n" r="K7">
-        <v>181978</v>
+        <v>190758</v>
       </c>
       <c t="inlineStr" r="L7">
         <is>
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c t="n" r="K8">
-        <v>16344</v>
+        <v>15972</v>
       </c>
       <c t="inlineStr" r="L8">
         <is>
@@ -858,7 +858,7 @@
         </is>
       </c>
       <c t="n" r="K9">
-        <v>106442</v>
+        <v>106272</v>
       </c>
       <c t="inlineStr" r="L9">
         <is>
@@ -934,7 +934,7 @@
         </is>
       </c>
       <c t="n" r="K10">
-        <v>3139</v>
+        <v>3091</v>
       </c>
       <c t="inlineStr" r="L10">
         <is>
@@ -1010,7 +1010,7 @@
         </is>
       </c>
       <c t="n" r="K11">
-        <v>25643</v>
+        <v>25485</v>
       </c>
       <c t="inlineStr" r="L11">
         <is>
@@ -1061,7 +1061,7 @@
       </c>
       <c t="inlineStr" r="E12">
         <is>
-          <t>JP1 JP2</t>
+          <t>JP1 JP2 JP3</t>
         </is>
       </c>
       <c t="inlineStr" r="F12">
@@ -1075,18 +1075,18 @@
         </is>
       </c>
       <c t="n" r="H12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c t="n" r="I12">
         <v>0.15000</v>
       </c>
       <c t="inlineStr" r="J12">
         <is>
-          <t>$0.30</t>
+          <t>$0.45</t>
         </is>
       </c>
       <c t="n" r="K12">
-        <v>17756</v>
+        <v>16627</v>
       </c>
       <c t="inlineStr" r="L12">
         <is>
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c t="n" r="K13">
-        <v>15875</v>
+        <v>15549</v>
       </c>
       <c t="inlineStr" r="L13">
         <is>
@@ -1236,7 +1236,7 @@
         </is>
       </c>
       <c t="n" r="K14">
-        <v>337750</v>
+        <v>335394</v>
       </c>
       <c t="inlineStr" r="L14">
         <is>
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c t="n" r="K15">
-        <v>5562</v>
+        <v>4556</v>
       </c>
       <c t="inlineStr" r="L15">
         <is>
@@ -1388,7 +1388,7 @@
         </is>
       </c>
       <c t="n" r="K16">
-        <v>14785</v>
+        <v>14782</v>
       </c>
       <c t="inlineStr" r="L16">
         <is>
@@ -1464,7 +1464,7 @@
         </is>
       </c>
       <c t="n" r="K17">
-        <v>4495</v>
+        <v>4392</v>
       </c>
       <c t="inlineStr" r="L17">
         <is>
@@ -1540,7 +1540,7 @@
         </is>
       </c>
       <c t="n" r="K18">
-        <v>3663</v>
+        <v>3660</v>
       </c>
       <c t="inlineStr" r="L18">
         <is>
@@ -1616,7 +1616,7 @@
         </is>
       </c>
       <c t="n" r="K19">
-        <v>791941</v>
+        <v>752201</v>
       </c>
       <c t="inlineStr" r="L19">
         <is>
@@ -1692,7 +1692,7 @@
         </is>
       </c>
       <c t="n" r="K20">
-        <v>1333942</v>
+        <v>1290726</v>
       </c>
       <c t="inlineStr" r="L20">
         <is>
@@ -1768,7 +1768,7 @@
         </is>
       </c>
       <c t="n" r="K21">
-        <v>1139</v>
+        <v>1124</v>
       </c>
       <c t="inlineStr" r="L21">
         <is>
@@ -1842,7 +1842,7 @@
         </is>
       </c>
       <c t="n" r="K22">
-        <v>199128</v>
+        <v>191048</v>
       </c>
       <c t="inlineStr" r="L22">
         <is>
@@ -1918,7 +1918,7 @@
         </is>
       </c>
       <c t="n" r="K23">
-        <v>3384</v>
+        <v>3378</v>
       </c>
       <c t="inlineStr" r="L23">
         <is>
@@ -1994,7 +1994,7 @@
         </is>
       </c>
       <c t="n" r="K24">
-        <v>676</v>
+        <v>657</v>
       </c>
       <c t="inlineStr" r="L24">
         <is>

</xml_diff>